<commit_message>
Changed: Lg Names Loading in scr loading Change Lg on Lg DD change
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/AngularJS App Doc.xlsx
+++ b/BballMVC/_Documentation/AngularJS App Doc.xlsx
@@ -1,38 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876336FC-E35A-47C3-9108-1253580EAFA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74CAA47-EECB-4E9C-8D75-66B7C7626476}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="435" windowWidth="22860" windowHeight="11445" activeTab="1" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
+    <workbookView xWindow="58905" yWindow="1680" windowWidth="27075" windowHeight="9120" activeTab="2" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Controllers" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Keith</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{8F8D2941-C12D-4CD4-B3EC-6BA29AE72BCF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>App/_Services</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{77C45071-C2F3-4C7F-884A-794656AEF3FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adjustments/UpdateYesterdaysAdjustments</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Folder</t>
   </si>
@@ -131,13 +165,73 @@
   </si>
   <si>
     <t>Update</t>
+  </si>
+  <si>
+    <t>Html</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Startup</t>
+  </si>
+  <si>
+    <t>Run.js</t>
+  </si>
+  <si>
+    <t>APIController</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>Sql Server</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>url: UrlUpdateYesterdaysAdjustments</t>
+  </si>
+  <si>
+    <t>UpdateYesterdaysAdjustments</t>
+  </si>
+  <si>
+    <t>uspUpdateYesterdaysAdjustments</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Refresh Matchups</t>
+  </si>
+  <si>
+    <t>RefreshTodaysMatchups()</t>
+  </si>
+  <si>
+    <t>TMController.js</t>
+  </si>
+  <si>
+    <t>UrlRefreshTodaysMatchups</t>
+  </si>
+  <si>
+    <t>/Data/RefreshMatchups</t>
+  </si>
+  <si>
+    <t>Data/RefreshMatchups</t>
+  </si>
+  <si>
+    <t>oDataBO.RefreshTodaysMatchups(oBballInfoDTO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +246,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -195,12 +302,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,6 +333,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>876301</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>17050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E1EC7EC-40F0-47C0-B29C-CBE508A17315}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266826" y="581026"/>
+          <a:ext cx="876300" cy="331374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF0AAC3-D700-42E8-8248-E782A3489850}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -706,4 +872,127 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E08A17A-8508-4836-BC47-C273B51CD5B5}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Put catch code in Data / RefreshTodaysMatchups method
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/AngularJS App Doc.xlsx
+++ b/BballMVC/_Documentation/AngularJS App Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0269DC-01EC-4B9D-AEC9-0FFE9ECECD16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0F449F-53F0-4D78-B3C7-3FCA49510E3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57765" yWindow="2850" windowWidth="24135" windowHeight="12705" activeTab="2" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
+    <workbookView xWindow="58275" yWindow="150" windowWidth="24135" windowHeight="12705" activeTab="2" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>Folder</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Data/RefreshTodaysMatchups</t>
+  </si>
+  <si>
+    <t>Select Game Date</t>
   </si>
 </sst>
 </file>
@@ -953,11 +956,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E08A17A-8508-4836-BC47-C273B51CD5B5}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,33 +1171,62 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>31</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>32</v>
+      </c>
       <c r="G16" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>33</v>
+      </c>
       <c r="G17" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>34</v>
+      </c>
       <c r="G18" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>35</v>
+      </c>
       <c r="G19" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>36</v>
+      </c>
       <c r="G20" s="4" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TM table adding Pts Allowed AppInit: Load BxScores & UpdateYesterdaysAdjustments
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/AngularJS App Doc.xlsx
+++ b/BballMVC/_Documentation/AngularJS App Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0F449F-53F0-4D78-B3C7-3FCA49510E3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A31E8DF-DBFF-4D15-92A6-D99AE0EF3CEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58275" yWindow="150" windowWidth="24135" windowHeight="12705" activeTab="2" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
+    <workbookView xWindow="59535" yWindow="1110" windowWidth="22350" windowHeight="13470" activeTab="2" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
   <si>
     <t>Folder</t>
   </si>
@@ -217,9 +217,6 @@
     <t>UrlRefreshTodaysMatchups</t>
   </si>
   <si>
-    <t>oDataBO.RefreshTodaysMatchups(oBballInfoDTO)</t>
-  </si>
-  <si>
     <t>SelectLeague()</t>
   </si>
   <si>
@@ -253,15 +250,6 @@
     <t>RotationDO.PopulateRotation(ocRotation, _oBballInfoDTO, _oLeagueDTO);</t>
   </si>
   <si>
-    <t>Data/GetLeagueData</t>
-  </si>
-  <si>
-    <t>GetLeagueData(IBballInfoDTO oBballInfoDTO)</t>
-  </si>
-  <si>
-    <t>GetLeagueData(oBballInfoDTO)</t>
-  </si>
-  <si>
     <t>Pop:</t>
   </si>
   <si>
@@ -274,20 +262,114 @@
     <t>ocTeams</t>
   </si>
   <si>
-    <t>if Yesterday, PGA</t>
-  </si>
-  <si>
     <t>Data/RefreshTodaysMatchups</t>
   </si>
   <si>
     <t>Select Game Date</t>
+  </si>
+  <si>
+    <t>UrlGetData</t>
+  </si>
+  <si>
+    <t>CollectionType:</t>
+  </si>
+  <si>
+    <t>GetLeagueData</t>
+  </si>
+  <si>
+    <t>Data/GetData</t>
+  </si>
+  <si>
+    <t>GetDataConstants.GetLeagueData</t>
+  </si>
+  <si>
+    <t>DataDO().GetLeagueData</t>
+  </si>
+  <si>
+    <t>uspQueryAdjustmentInfo</t>
+  </si>
+  <si>
+    <t>GetAdjustmentInfo</t>
+  </si>
+  <si>
+    <t>DataDO.GetLeagueData</t>
+  </si>
+  <si>
+    <r>
+      <t>AdjustmentsDO.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GetAdjustmentInfo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TodaysMatchupsDO(oBballInfoDTO).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GetTodaysMatchups</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RefreshPostGameAnalysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(oBballInfoDTO);</t>
+    </r>
+  </si>
+  <si>
+    <t>ExecuteStoredProcedureNonQuery</t>
+  </si>
+  <si>
+    <t>uspCalcTodaysMatchups</t>
+  </si>
+  <si>
+    <t>TodaysMatchupsDO.GetTodaysMatchups</t>
+  </si>
+  <si>
+    <t>oDataBO.GetData(oBballInfoDTO)</t>
+  </si>
+  <si>
+    <t>"RefreshTodaysMatchups"</t>
+  </si>
+  <si>
+    <t>GetDailySummaryDTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +408,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -397,6 +495,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,11 +1062,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E08A17A-8508-4836-BC47-C273B51CD5B5}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +1076,8 @@
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
     <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1042,7 +1149,7 @@
         <v>48</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>31</v>
@@ -1062,7 +1169,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1072,11 +1179,11 @@
       <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>50</v>
+      <c r="E6" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1084,148 +1191,255 @@
         <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8" s="5"/>
+      <c r="E8"/>
+      <c r="F8" s="10" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="F10" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D11" s="5"/>
       <c r="F11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D12" s="5"/>
       <c r="F12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>15</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>30</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="G22" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="G23" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>31</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>32</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>33</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>34</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>35</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>36</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed RotNum = zero problem
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/AngularJS App Doc.xlsx
+++ b/BballMVC/_Documentation/AngularJS App Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211A7B3B-EEDE-4FDC-8ED6-CC6F93F60FFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE59A1C9-C68A-4B56-968F-92AB96D5FAB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59310" yWindow="2280" windowWidth="22815" windowHeight="11835" activeTab="2" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
+    <workbookView xWindow="59340" yWindow="2250" windowWidth="22815" windowHeight="11835" activeTab="2" xr2:uid="{4DF0F12C-FB7F-4D2E-92E5-73A3C6910D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="111">
   <si>
     <t>Folder</t>
   </si>
@@ -412,12 +412,83 @@
   <si>
     <t>GetaData</t>
   </si>
+  <si>
+    <t>In TMs - ADJs by Tm</t>
+  </si>
+  <si>
+    <t>_TodaysMatchupsTable</t>
+  </si>
+  <si>
+    <t>OpenAdjustmentsByTeamModal</t>
+  </si>
+  <si>
+    <t>TodaysMatchupsController</t>
+  </si>
+  <si>
+    <t>$scope.$broadcast('OpenAdjustmentsByTeamEvent', Team, SideLine);</t>
+  </si>
+  <si>
+    <t>AdjustmentsByTeamModalController</t>
+  </si>
+  <si>
+    <t>ajx.AjaxGet(url.UrlGetAdjustmentsByTeam</t>
+  </si>
+  <si>
+    <t>$rootScope GameDate LeagueName</t>
+  </si>
+  <si>
+    <t>Team, SideLine</t>
+  </si>
+  <si>
+    <t>GetAdjustmentsByTeam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GameDate LeagueName
+Team, SideLine</t>
+  </si>
+  <si>
+    <t>GetTodaysAdjustmentsByTeam</t>
+  </si>
+  <si>
+    <t>AdjustmentsBO</t>
+  </si>
+  <si>
+    <t>AdjustmentController</t>
+  </si>
+  <si>
+    <t>AdjustmentsDO</t>
+  </si>
+  <si>
+    <t>uspQueryAdjustmentsByTeam</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OpenAdjustmentsByTeamModal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Team, SideLine)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +553,27 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -524,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -562,13 +654,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,17 +1228,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E08A17A-8508-4836-BC47-C273B51CD5B5}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
@@ -1222,14 +1322,14 @@
     </row>
     <row r="5" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1519,34 +1619,120 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
         <v>33</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>35</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>36</v>
       </c>
+      <c r="D31" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>37</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>38</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>39</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>40</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>